<commit_message>
maj data et resultas
</commit_message>
<xml_diff>
--- a/data/charge_virale_groupe.xlsx
+++ b/data/charge_virale_groupe.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/JM/NanoString/NanoString_Covid/nanostring_covid/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/JM/NanoString/IFN_covid_nano/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101773BA-7D70-114A-B3DB-3995F429B4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C624A11-B313-E849-BBE4-F33DAF15DB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27560" windowHeight="16940" xr2:uid="{CD9F84F5-3B8F-6B47-988D-C2CEB9BE8E8F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="66">
   <si>
     <t>patient</t>
   </si>
@@ -64,9 +64,6 @@
     <t>charge_virale</t>
   </si>
   <si>
-    <t>Groupe</t>
-  </si>
-  <si>
     <t>20201230_COVIDAURA#01_BJ-0116-V1_05.RCC</t>
   </si>
   <si>
@@ -224,6 +221,21 @@
   </si>
   <si>
     <t>charge_virale_log10</t>
+  </si>
+  <si>
+    <t>Reponse</t>
+  </si>
+  <si>
+    <t>NR-</t>
+  </si>
+  <si>
+    <t>RP-</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -594,7 +606,7 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,7 +620,7 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -634,33 +646,33 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -672,28 +684,28 @@
         <f>10^H2</f>
         <v>15848931.924611172</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>20</v>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -705,28 +717,28 @@
         <f>10^H3</f>
         <v>316227.7660168382</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
+      <c r="J3" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1">
         <v>3</v>
@@ -738,28 +750,28 @@
         <f>10^H4</f>
         <v>1258.925411794168</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>20</v>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
@@ -770,28 +782,28 @@
       <c r="I5" s="2">
         <v>100000000</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>52</v>
+      <c r="J5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1">
         <v>5</v>
@@ -803,28 +815,28 @@
         <f>10^H6</f>
         <v>125892541.17941682</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>20</v>
+      <c r="J6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
         <v>6</v>
@@ -835,28 +847,28 @@
       <c r="I7" s="2">
         <v>5011872.3362727314</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>52</v>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1">
         <v>7</v>
@@ -868,28 +880,28 @@
         <f>10^H8</f>
         <v>630.95734448019323</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>20</v>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1">
         <v>8</v>
@@ -901,28 +913,28 @@
         <f>10^H9</f>
         <v>630957344.48019624</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1">
         <v>9</v>
@@ -934,28 +946,28 @@
         <f>10^H10</f>
         <v>79432.823472428237</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>20</v>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1">
         <v>10</v>
@@ -966,28 +978,28 @@
       <c r="I11" s="2">
         <v>3162277.6601683851</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>52</v>
+      <c r="J11" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1">
         <v>11</v>
@@ -999,28 +1011,28 @@
         <f>10^H12</f>
         <v>6309573.4448019378</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>20</v>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1">
         <v>12</v>
@@ -1032,28 +1044,28 @@
         <f>10^H13</f>
         <v>2511.8864315095811</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>20</v>
+      <c r="J13" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>
@@ -1065,28 +1077,28 @@
         <f>10^H14</f>
         <v>2511.8864315095811</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>14</v>
+      <c r="J14" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="1">
         <v>14</v>
@@ -1098,28 +1110,28 @@
         <f>10^H15</f>
         <v>1258925.4117941677</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>20</v>
+      <c r="J15" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1">
         <v>15</v>
@@ -1130,28 +1142,28 @@
       <c r="I16" s="2">
         <v>31622776.601683889</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>52</v>
+      <c r="J16" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1">
         <v>16</v>
@@ -1163,28 +1175,28 @@
         <f>10^H17</f>
         <v>79432823.472428367</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>20</v>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3">
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G18" s="1">
         <v>17</v>
@@ -1196,28 +1208,28 @@
         <f>10^H18</f>
         <v>19952.623149688792</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>20</v>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1">
         <v>18</v>
@@ -1229,28 +1241,28 @@
         <f>10^H19</f>
         <v>1258.925411794168</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>20</v>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="1">
         <v>19</v>
@@ -1262,28 +1274,28 @@
         <f>10^H20</f>
         <v>1584893.1924611153</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>20</v>
+      <c r="J20" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G21" s="1">
         <v>20</v>
@@ -1295,28 +1307,28 @@
         <f>10^H21</f>
         <v>10000000</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>20</v>
+      <c r="J21" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G22" s="1">
         <v>21</v>
@@ -1327,28 +1339,28 @@
       <c r="I22" s="2">
         <v>50118723.362727284</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>52</v>
+      <c r="J22" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="1">
         <v>22</v>
@@ -1360,28 +1372,28 @@
         <f>10^H23</f>
         <v>794328.23472428333</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>20</v>
+      <c r="J23" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24" s="1">
         <v>23</v>
@@ -1393,28 +1405,28 @@
         <f>10^H24</f>
         <v>251188.64315095844</v>
       </c>
-      <c r="J24" s="2" t="s">
-        <v>20</v>
+      <c r="J24" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" s="1">
         <v>25</v>
@@ -1426,28 +1438,28 @@
         <f>10^H25</f>
         <v>7943282.3472428275</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>20</v>
+      <c r="J25" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G26" s="1">
         <v>26</v>
@@ -1458,28 +1470,28 @@
       <c r="I26" s="2">
         <v>12589254.117941668</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>52</v>
+      <c r="J26" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G27" s="1">
         <v>27</v>
@@ -1491,28 +1503,28 @@
         <f>10^H27</f>
         <v>794328.23472428333</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>20</v>
+      <c r="J27" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G28" s="1">
         <v>29</v>
@@ -1523,28 +1535,28 @@
       <c r="I28" s="2">
         <v>5011.8723362727324</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>52</v>
+      <c r="J28" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29" s="1">
         <v>30</v>
@@ -1556,28 +1568,28 @@
         <f>10^H29</f>
         <v>1584893.1924611153</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>20</v>
+      <c r="J29" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30" s="1">
         <v>31</v>
@@ -1589,28 +1601,28 @@
         <f>10^H30</f>
         <v>19952623.149688821</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>20</v>
+      <c r="J30" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G31" s="1">
         <v>47</v>
@@ -1622,28 +1634,28 @@
         <f>10^H31</f>
         <v>1186.0070191327995</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>20</v>
+      <c r="J31" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="1">
         <v>2</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G32" s="1">
         <v>48</v>
@@ -1654,28 +1666,28 @@
       <c r="I32" s="2">
         <v>70711409.395973176</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>52</v>
+      <c r="J32" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="1">
         <v>2</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33" s="1">
         <v>49</v>
@@ -1684,31 +1696,31 @@
         <v>1.1777778954922942</v>
       </c>
       <c r="I33" s="2">
-        <f>10^H33</f>
+        <f t="shared" ref="I33:I41" si="0">10^H33</f>
         <v>15.058367624333627</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>14</v>
+      <c r="J33" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1">
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G34" s="1">
         <v>50</v>
@@ -1717,31 +1729,31 @@
         <v>2.8696146801390481</v>
       </c>
       <c r="I34" s="2">
-        <f>10^H34</f>
+        <f t="shared" si="0"/>
         <v>740.65281899109868</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>14</v>
+      <c r="J34" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1">
         <v>4</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G35" s="1">
         <v>51</v>
@@ -1750,31 +1762,31 @@
         <v>6.9614275722544114</v>
       </c>
       <c r="I35" s="2">
-        <f>10^H35</f>
+        <f t="shared" si="0"/>
         <v>9150136.4877161216</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>20</v>
+      <c r="J35" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G36" s="1">
         <v>52</v>
@@ -1783,31 +1795,31 @@
         <v>7.3137010890980712</v>
       </c>
       <c r="I36" s="2">
-        <f>10^H36</f>
+        <f t="shared" si="0"/>
         <v>20592121.360411145</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>20</v>
+      <c r="J36" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="1">
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G37" s="1">
         <v>54</v>
@@ -1816,31 +1828,31 @@
         <v>8.82</v>
       </c>
       <c r="I37" s="2">
-        <f>10^H37</f>
+        <f t="shared" si="0"/>
         <v>660693448.00759673</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>20</v>
+      <c r="J37" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G38" s="1">
         <v>56</v>
@@ -1849,31 +1861,31 @@
         <v>6.6005403390034578</v>
       </c>
       <c r="I38" s="2">
-        <f>10^H38</f>
+        <f t="shared" si="0"/>
         <v>3986027.94411179</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>20</v>
+      <c r="J38" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G39" s="1">
         <v>58</v>
@@ -1882,31 +1894,31 @@
         <v>6.3040743736066949</v>
       </c>
       <c r="I39" s="2">
-        <f>10^H39</f>
+        <f t="shared" si="0"/>
         <v>2014069.1328077675</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>20</v>
+      <c r="J39" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1">
         <v>2</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G40" s="1">
         <v>59</v>
@@ -1915,31 +1927,31 @@
         <v>7.7105777950287537</v>
       </c>
       <c r="I40" s="2">
-        <f>10^H40</f>
+        <f t="shared" si="0"/>
         <v>51354416.026206508</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>20</v>
+      <c r="J40" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" s="1">
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G41" s="1">
         <v>60</v>
@@ -1948,31 +1960,31 @@
         <v>7.7395326971077854</v>
       </c>
       <c r="I41" s="2">
-        <f>10^H41</f>
+        <f t="shared" si="0"/>
         <v>54894988.332037121</v>
       </c>
-      <c r="J41" s="2" t="s">
-        <v>14</v>
+      <c r="J41" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1">
         <v>3</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G42" s="1">
         <v>61</v>
@@ -1983,28 +1995,28 @@
       <c r="I42" s="2">
         <v>8285812.4355891598</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>52</v>
+      <c r="J42" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1">
         <v>5</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G43" s="1">
         <v>62</v>
@@ -2016,28 +2028,28 @@
         <f>10^H43</f>
         <v>74709.851551956832</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>14</v>
+      <c r="J43" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1">
         <v>2</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G44" s="1">
         <v>63</v>
@@ -2049,28 +2061,28 @@
         <f>10^H44</f>
         <v>67165071.770334959</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>20</v>
+      <c r="J44" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1">
         <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G45" s="1">
         <v>64</v>
@@ -2082,13 +2094,13 @@
         <f>10^H45</f>
         <v>905615576.39795935</v>
       </c>
-      <c r="J45" s="2" t="s">
-        <v>20</v>
+      <c r="J45" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{ADC88C41-6C86-2449-8979-5477D82B798A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J45">
+  <autoFilter ref="A1:I1" xr:uid="{ADC88C41-6C86-2449-8979-5477D82B798A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I45">
       <sortCondition ref="G1:G45"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
:ajout des resultats avec signature VT1vsT + suppression des fichiers
</commit_message>
<xml_diff>
--- a/data/charge_virale_groupe.xlsx
+++ b/data/charge_virale_groupe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/JM/NanoString/IFN_covid_nano/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C624A11-B313-E849-BBE4-F33DAF15DB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F381001-89B6-BA4E-B79E-3A174934F2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27560" windowHeight="16940" xr2:uid="{CD9F84F5-3B8F-6B47-988D-C2CEB9BE8E8F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29120" windowHeight="18880" xr2:uid="{CD9F84F5-3B8F-6B47-988D-C2CEB9BE8E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="67">
   <si>
     <t>patient</t>
   </si>
@@ -236,13 +236,16 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>numero_patient_victor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,16 +260,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -274,11 +306,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,6 +347,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -603,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC88C41-6C86-2449-8979-5477D82B798A}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="138" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,10 +701,13 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,11 +735,20 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -684,11 +777,20 @@
         <f>10^H2</f>
         <v>15848931.924611172</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="7">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -717,11 +819,20 @@
         <f>10^H3</f>
         <v>316227.7660168382</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="5">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="7">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -750,11 +861,20 @@
         <f>10^H4</f>
         <v>1258.925411794168</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="5">
+        <v>3</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="7">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -782,11 +902,20 @@
       <c r="I5" s="2">
         <v>100000000</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="5">
+        <v>4</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -815,11 +944,20 @@
         <f>10^H6</f>
         <v>125892541.17941682</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="5">
+        <v>5</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="7">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -847,11 +985,20 @@
       <c r="I7" s="2">
         <v>5011872.3362727314</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="5">
+        <v>6</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="7">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -880,11 +1027,20 @@
         <f>10^H8</f>
         <v>630.95734448019323</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="5">
+        <v>7</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="7">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -913,11 +1069,20 @@
         <f>10^H9</f>
         <v>630957344.48019624</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="5">
+        <v>8</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -946,11 +1111,20 @@
         <f>10^H10</f>
         <v>79432.823472428237</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="5">
+        <v>9</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
@@ -978,11 +1152,20 @@
       <c r="I11" s="2">
         <v>3162277.6601683851</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="5">
+        <v>10</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="7">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -1011,11 +1194,20 @@
         <f>10^H12</f>
         <v>6309573.4448019378</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="5">
+        <v>11</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="7">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1044,11 +1236,20 @@
         <f>10^H13</f>
         <v>2511.8864315095811</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="5">
+        <v>12</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="7">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1077,11 +1278,20 @@
         <f>10^H14</f>
         <v>2511.8864315095811</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="5">
+        <v>13</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="7">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1110,11 +1320,20 @@
         <f>10^H15</f>
         <v>1258925.4117941677</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="5">
+        <v>14</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="7">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -1142,11 +1361,20 @@
       <c r="I16" s="2">
         <v>31622776.601683889</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="5">
+        <v>15</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="7">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1175,11 +1403,20 @@
         <f>10^H17</f>
         <v>79432823.472428367</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="5">
+        <v>16</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="7">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -1208,11 +1445,20 @@
         <f>10^H18</f>
         <v>19952.623149688792</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="5">
+        <v>17</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="7">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1241,11 +1487,20 @@
         <f>10^H19</f>
         <v>1258.925411794168</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="5">
+        <v>18</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="7">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1274,11 +1529,20 @@
         <f>10^H20</f>
         <v>1584893.1924611153</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="5">
+        <v>19</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M20" s="7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1307,11 +1571,20 @@
         <f>10^H21</f>
         <v>10000000</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="5">
+        <v>20</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -1339,11 +1612,20 @@
       <c r="I22" s="2">
         <v>50118723.362727284</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="5">
+        <v>21</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="7">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1372,11 +1654,20 @@
         <f>10^H23</f>
         <v>794328.23472428333</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" s="5">
+        <v>22</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1405,11 +1696,20 @@
         <f>10^H24</f>
         <v>251188.64315095844</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="5">
+        <v>23</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1438,11 +1738,20 @@
         <f>10^H25</f>
         <v>7943282.3472428275</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="5">
+        <v>25</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="7">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>56</v>
       </c>
@@ -1470,11 +1779,20 @@
       <c r="I26" s="2">
         <v>12589254.117941668</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="5">
+        <v>26</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M26" s="7">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
@@ -1503,11 +1821,20 @@
         <f>10^H27</f>
         <v>794328.23472428333</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="5">
+        <v>27</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M27" s="7">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>57</v>
       </c>
@@ -1535,11 +1862,20 @@
       <c r="I28" s="2">
         <v>5011.8723362727324</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="5">
+        <v>29</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M28" s="7">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -1568,11 +1904,20 @@
         <f>10^H29</f>
         <v>1584893.1924611153</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" s="5">
+        <v>30</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29" s="7">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
@@ -1601,11 +1946,20 @@
         <f>10^H30</f>
         <v>19952623.149688821</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="5">
+        <v>31</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="7">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
@@ -1634,11 +1988,20 @@
         <f>10^H31</f>
         <v>1186.0070191327995</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="5">
+        <v>47</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="7">
+        <v>3.0740872593162889</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1666,11 +2029,20 @@
       <c r="I32" s="2">
         <v>70711409.395973176</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J32" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="5">
+        <v>48</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M32" s="7">
+        <v>7.8494894940000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -1699,11 +2071,20 @@
         <f t="shared" ref="I33:I41" si="0">10^H33</f>
         <v>15.058367624333627</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="J33" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="5">
+        <v>49</v>
+      </c>
+      <c r="L33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1.17777789549229</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -1732,11 +2113,20 @@
         <f t="shared" si="0"/>
         <v>740.65281899109868</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="J34" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="5">
+        <v>50</v>
+      </c>
+      <c r="L34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="7">
+        <v>2.8696146800000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
@@ -1765,11 +2155,20 @@
         <f t="shared" si="0"/>
         <v>9150136.4877161216</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="K35" s="5">
+        <v>51</v>
+      </c>
+      <c r="L35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M35" s="7">
+        <v>6.9614275722544114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1798,11 +2197,20 @@
         <f t="shared" si="0"/>
         <v>20592121.360411145</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J36" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="5">
+        <v>52</v>
+      </c>
+      <c r="L36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M36" s="7">
+        <v>7.3137010890980712</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1831,11 +2239,20 @@
         <f t="shared" si="0"/>
         <v>660693448.00759673</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="5">
+        <v>54</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="7">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1864,11 +2281,20 @@
         <f t="shared" si="0"/>
         <v>3986027.94411179</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="J38" s="8" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="5">
+        <v>56</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38" s="7">
+        <v>6.6005403390034596</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1897,11 +2323,20 @@
         <f t="shared" si="0"/>
         <v>2014069.1328077675</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="5">
+        <v>58</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="7">
+        <v>6.3040743736066949</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1930,11 +2365,20 @@
         <f t="shared" si="0"/>
         <v>51354416.026206508</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="5">
+        <v>59</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M40" s="7">
+        <v>7.7105777950287537</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>15</v>
       </c>
@@ -1963,11 +2407,20 @@
         <f t="shared" si="0"/>
         <v>54894988.332037121</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J41" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="5">
+        <v>60</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="M41" s="7">
+        <v>7.7395326971077898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1995,11 +2448,20 @@
       <c r="I42" s="2">
         <v>8285812.4355891598</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="5">
+        <v>61</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M42" s="7">
+        <v>6.918335098</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -2028,11 +2490,20 @@
         <f>10^H43</f>
         <v>74709.851551956832</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="5">
+        <v>62</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M43" s="7">
+        <v>4.8733778734693729</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -2061,11 +2532,20 @@
         <f>10^H44</f>
         <v>67165071.770334959</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44" s="5">
+        <v>63</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M44" s="7">
+        <v>7.8271434830000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -2094,9 +2574,24 @@
         <f>10^H45</f>
         <v>905615576.39795935</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="J45" s="8" t="s">
         <v>64</v>
       </c>
+      <c r="K45" s="5">
+        <v>64</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M45" s="7">
+        <v>8.9569438836824293</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J46" s="8"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{ADC88C41-6C86-2449-8979-5477D82B798A}">

</xml_diff>